<commit_message>
adding new DETECTR notebooks
</commit_message>
<xml_diff>
--- a/tidy_data/DETECTR_028_Luciferase_tidy_metadata.xlsx
+++ b/tidy_data/DETECTR_028_Luciferase_tidy_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Amy_Lyden_CZBiohub/DETECTR/github/DETECTR/tidy_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CFA79A81-DBBE-FA4D-8A58-B0654150D686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2C4817C4-6F7B-4342-B6B7-640214C0B9B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="3860" windowWidth="26440" windowHeight="15440" activeTab="1"/>
+    <workbookView xWindow="1340" yWindow="1720" windowWidth="26440" windowHeight="15440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DETECTR_028_Luciferase_tidy_met" sheetId="1" r:id="rId1"/>
@@ -810,80 +810,62 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Standard Curve'!$G$2:$G$25</c:f>
+              <c:f>'Standard Curve'!$G$8:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>0.3125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5</c:v>
+                  <c:v>0.3125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.25</c:v>
+                  <c:v>0.15625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.25</c:v>
+                  <c:v>0.15625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.625</c:v>
+                  <c:v>7.8125E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.625</c:v>
+                  <c:v>7.8125E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3125</c:v>
+                  <c:v>3.90625E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.3125</c:v>
+                  <c:v>3.90625E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.15625</c:v>
+                  <c:v>1.9531199999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.15625</c:v>
+                  <c:v>1.9531199999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.8125E-2</c:v>
+                  <c:v>9.7655999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.8125E-2</c:v>
+                  <c:v>9.7655999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.90625E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.90625E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.9531199999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.9531199999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9.7655999999999993E-3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.7655999999999993E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -891,80 +873,62 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Standard Curve'!$H$2:$H$25</c:f>
+              <c:f>'Standard Curve'!$H$8:$H$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2784.239</c:v>
+                  <c:v>369.66699999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2631.6779999999999</c:v>
+                  <c:v>278.71699999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1396.52</c:v>
+                  <c:v>88.016000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1443.462</c:v>
+                  <c:v>117.355</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>707.06200000000001</c:v>
+                  <c:v>85.081999999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>677.72299999999996</c:v>
+                  <c:v>52.81</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>369.66699999999997</c:v>
+                  <c:v>161.363</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>278.71699999999998</c:v>
+                  <c:v>49.875999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>88.016000000000005</c:v>
+                  <c:v>70.412999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>117.355</c:v>
+                  <c:v>32.273000000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>85.081999999999994</c:v>
+                  <c:v>58.677</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>52.81</c:v>
+                  <c:v>26.405000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>161.363</c:v>
+                  <c:v>32.273000000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>49.875999999999998</c:v>
+                  <c:v>29.338999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70.412999999999997</c:v>
+                  <c:v>29.338999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32.273000000000003</c:v>
+                  <c:v>41.073999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>58.677</c:v>
+                  <c:v>17.602999999999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26.405000000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>32.273000000000003</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>29.338999999999999</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>29.338999999999999</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>41.073999999999998</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>17.602999999999899</c:v>
-                </c:pt>
-                <c:pt idx="23">
                   <c:v>23.471</c:v>
                 </c:pt>
               </c:numCache>
@@ -13878,7 +13842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8:L9"/>
     </sheetView>
   </sheetViews>

</xml_diff>